<commit_message>
updates to the slicing coordinates in the xlsx files
</commit_message>
<xml_diff>
--- a/VULCAN/VulcanSlicingCoords.xlsx
+++ b/VULCAN/VulcanSlicingCoords.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Boller CFD\AVIATION CFD\output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75B2DF1F-D1D0-4714-9688-D9423B256519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68D01D93-6130-4EA4-8FCF-89808CEF9004}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-5685" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -146,7 +145,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -162,6 +161,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -171,7 +178,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -473,11 +480,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -544,6 +562,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -551,6 +572,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -836,47 +860,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:V24"/>
+  <dimension ref="B1:W24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="U13" sqref="U13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="19" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="14" max="17" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="24" t="s">
+    <row r="1" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="G2" s="25" t="s">
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="G2" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
-      <c r="N2" s="26"/>
-      <c r="O2" s="26"/>
-      <c r="P2" s="26"/>
-      <c r="Q2" s="26"/>
-      <c r="R2" s="26"/>
-      <c r="S2" s="27"/>
-      <c r="V2" s="3" t="s">
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
+      <c r="N2" s="27"/>
+      <c r="O2" s="27"/>
+      <c r="P2" s="27"/>
+      <c r="Q2" s="27"/>
+      <c r="R2" s="27"/>
+      <c r="S2" s="28"/>
+      <c r="T2" s="29"/>
+      <c r="W2" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -923,13 +955,16 @@
         <v>1</v>
       </c>
       <c r="S3" s="5">
-        <v>2</v>
-      </c>
-      <c r="V3" s="21" t="s">
+        <v>1.2</v>
+      </c>
+      <c r="T3" s="24">
+        <v>2.33</v>
+      </c>
+      <c r="W3" s="21" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
@@ -976,13 +1011,16 @@
         <v>0.53164999999999996</v>
       </c>
       <c r="S4" s="9">
+        <v>0.54528460000000001</v>
+      </c>
+      <c r="T4" s="9">
         <v>0.62218374399999998</v>
       </c>
-      <c r="V4" s="21" t="s">
+      <c r="W4" s="21" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1029,13 +1067,16 @@
         <v>-1.5304E-2</v>
       </c>
       <c r="S5" s="13">
+        <v>-1.0340999999999999E-2</v>
+      </c>
+      <c r="T5" s="13">
         <v>-1.0253E-2</v>
       </c>
-      <c r="V5" s="21" t="s">
+      <c r="W5" s="21" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:23" x14ac:dyDescent="0.3">
       <c r="G6" s="10" t="s">
         <v>9</v>
       </c>
@@ -1075,11 +1116,14 @@
       <c r="S6" s="13">
         <v>1.2699999999999999E-2</v>
       </c>
-      <c r="V6" s="21" t="s">
+      <c r="T6" s="13">
+        <v>1.2699999999999999E-2</v>
+      </c>
+      <c r="W6" s="21" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="1" t="s">
         <v>31</v>
       </c>
@@ -1120,13 +1164,16 @@
         <v>0.53164999999999996</v>
       </c>
       <c r="S7" s="17">
+        <v>0.54528460000000001</v>
+      </c>
+      <c r="T7" s="17">
         <v>0.62218374399999998</v>
       </c>
-      <c r="V7" s="22" t="s">
+      <c r="W7" s="22" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
         <v>32</v>
       </c>
@@ -1173,10 +1220,13 @@
         <v>2.1881999999999999E-2</v>
       </c>
       <c r="S8" s="17">
+        <v>2.6844999999999997E-2</v>
+      </c>
+      <c r="T8" s="17">
         <v>2.6932999999999999E-2</v>
       </c>
     </row>
-    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:23" x14ac:dyDescent="0.3">
       <c r="G9" s="14" t="s">
         <v>12</v>
       </c>
@@ -1216,8 +1266,11 @@
       <c r="S9" s="17">
         <v>1.2699999999999999E-2</v>
       </c>
+      <c r="T9" s="17">
+        <v>1.2699999999999999E-2</v>
+      </c>
     </row>
-    <row r="10" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G10" s="18" t="s">
         <v>13</v>
       </c>
@@ -1257,29 +1310,33 @@
       <c r="S10" s="19">
         <v>500</v>
       </c>
+      <c r="T10" s="19">
+        <v>500</v>
+      </c>
     </row>
-    <row r="17" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="G17" s="24" t="s">
+    <row r="17" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="G17" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="H17" s="24"/>
-      <c r="I17" s="24"/>
-      <c r="J17" s="24"/>
-      <c r="K17" s="24"/>
-      <c r="L17" s="24"/>
-      <c r="M17" s="24"/>
-      <c r="N17" s="24"/>
-      <c r="O17" s="24"/>
-      <c r="P17" s="24"/>
-      <c r="Q17" s="24"/>
-      <c r="R17" s="24"/>
-      <c r="S17" s="24"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="25"/>
+      <c r="J17" s="25"/>
+      <c r="K17" s="25"/>
+      <c r="L17" s="25"/>
+      <c r="M17" s="25"/>
+      <c r="N17" s="25"/>
+      <c r="O17" s="25"/>
+      <c r="P17" s="25"/>
+      <c r="Q17" s="25"/>
+      <c r="R17" s="25"/>
+      <c r="S17" s="25"/>
+      <c r="T17" s="25"/>
     </row>
-    <row r="18" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B18" s="24" t="s">
+    <row r="18" spans="2:20" x14ac:dyDescent="0.3">
+      <c r="B18" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="24"/>
+      <c r="C18" s="25"/>
       <c r="E18" t="s">
         <v>21</v>
       </c>
@@ -1323,10 +1380,13 @@
         <v>1</v>
       </c>
       <c r="S18">
+        <v>1.2</v>
+      </c>
+      <c r="T18">
         <v>2.3279999999999998</v>
       </c>
     </row>
-    <row r="19" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:20" x14ac:dyDescent="0.3">
       <c r="E19" t="s">
         <v>23</v>
       </c>
@@ -1341,7 +1401,7 @@
         <v>0.32713099999999995</v>
       </c>
       <c r="I19">
-        <f t="shared" ref="I19:S19" si="0">$F$18+(I18*$C$3)</f>
+        <f t="shared" ref="I19:T19" si="0">$F$18+(I18*$C$3)</f>
         <v>0.39530399999999999</v>
       </c>
       <c r="J19">
@@ -1380,12 +1440,16 @@
         <f t="shared" si="0"/>
         <v>0.53164999999999996</v>
       </c>
-      <c r="S19">
+      <c r="S19" s="23">
+        <f t="shared" si="0"/>
+        <v>0.54528460000000001</v>
+      </c>
+      <c r="T19">
         <f t="shared" si="0"/>
         <v>0.62218374399999998</v>
       </c>
     </row>
-    <row r="20" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:20" x14ac:dyDescent="0.3">
       <c r="G20" s="1" t="s">
         <v>25</v>
       </c>
@@ -1423,10 +1487,13 @@
         <v>-1.5304E-2</v>
       </c>
       <c r="S20" s="23">
+        <v>-1.0340999999999999E-2</v>
+      </c>
+      <c r="T20" s="23">
         <v>-1.0253E-2</v>
       </c>
     </row>
-    <row r="21" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:20" x14ac:dyDescent="0.3">
       <c r="G21" s="1" t="s">
         <v>26</v>
       </c>
@@ -1466,8 +1533,11 @@
       <c r="S21">
         <v>1.2699999999999999E-2</v>
       </c>
+      <c r="T21">
+        <v>1.2699999999999999E-2</v>
+      </c>
     </row>
-    <row r="22" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:20" x14ac:dyDescent="0.3">
       <c r="G22" s="1" t="s">
         <v>27</v>
       </c>
@@ -1476,7 +1546,7 @@
         <v>0.32713099999999995</v>
       </c>
       <c r="I22">
-        <f t="shared" ref="I22:S22" si="1">I19</f>
+        <f t="shared" ref="I22:T22" si="1">I19</f>
         <v>0.39530399999999999</v>
       </c>
       <c r="J22">
@@ -1516,11 +1586,15 @@
         <v>0.53164999999999996</v>
       </c>
       <c r="S22">
+        <f t="shared" ref="S22" si="2">S19</f>
+        <v>0.54528460000000001</v>
+      </c>
+      <c r="T22">
         <f t="shared" si="1"/>
         <v>0.62218374399999998</v>
       </c>
     </row>
-    <row r="23" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:20" x14ac:dyDescent="0.3">
       <c r="G23" s="1" t="s">
         <v>28</v>
       </c>
@@ -1529,51 +1603,55 @@
         <v>3.7185999999999997E-2</v>
       </c>
       <c r="I23">
-        <f t="shared" ref="I23:S23" si="2">I20+$F$19</f>
+        <f t="shared" ref="I23:T23" si="3">I20+$F$19</f>
         <v>3.6838999999999997E-2</v>
       </c>
       <c r="J23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3.5349999999999999E-2</v>
       </c>
       <c r="K23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.5386999999999998E-2</v>
       </c>
       <c r="L23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.4969999999999997E-2</v>
       </c>
       <c r="M23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.4582999999999995E-2</v>
       </c>
       <c r="N23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.4135999999999996E-2</v>
       </c>
       <c r="O23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.3719999999999996E-2</v>
       </c>
       <c r="P23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.5181999999999998E-2</v>
       </c>
       <c r="Q23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.8407999999999997E-2</v>
       </c>
       <c r="R23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.1881999999999999E-2</v>
       </c>
       <c r="S23">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="S23" si="4">S20+$F$19</f>
+        <v>2.6844999999999997E-2</v>
+      </c>
+      <c r="T23">
+        <f t="shared" si="3"/>
         <v>2.6932999999999999E-2</v>
       </c>
     </row>
-    <row r="24" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:20" x14ac:dyDescent="0.3">
       <c r="G24" s="1" t="s">
         <v>29</v>
       </c>
@@ -1582,55 +1660,59 @@
         <v>1.2699999999999999E-2</v>
       </c>
       <c r="I24">
-        <f t="shared" ref="I24:S24" si="3">I21</f>
+        <f t="shared" ref="I24:T24" si="5">I21</f>
         <v>1.2699999999999999E-2</v>
       </c>
       <c r="J24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.2699999999999999E-2</v>
       </c>
       <c r="K24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.2699999999999999E-2</v>
       </c>
       <c r="L24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.2699999999999999E-2</v>
       </c>
       <c r="M24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.2699999999999999E-2</v>
       </c>
       <c r="N24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.2699999999999999E-2</v>
       </c>
       <c r="O24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.2699999999999999E-2</v>
       </c>
       <c r="P24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.2699999999999999E-2</v>
       </c>
       <c r="Q24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.2699999999999999E-2</v>
       </c>
       <c r="R24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>1.2699999999999999E-2</v>
       </c>
       <c r="S24">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="S24" si="6">S21</f>
+        <v>1.2699999999999999E-2</v>
+      </c>
+      <c r="T24">
+        <f t="shared" si="5"/>
         <v>1.2699999999999999E-2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="B2:D2"/>
-    <mergeCell ref="G2:S2"/>
-    <mergeCell ref="G17:S17"/>
+    <mergeCell ref="G2:T2"/>
+    <mergeCell ref="G17:T17"/>
     <mergeCell ref="B18:C18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>